<commit_message>
add results for different s-values #24
- formulate set_up.m and run_all.m to loop over many s-values
- end loop early in apply_gains.m
- plotting sucess rates at different s-values (plot_svalues.m)
- increase marker size in plot_poles.m
</commit_message>
<xml_diff>
--- a/svalues.xlsx
+++ b/svalues.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\MastersMATLAB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAJP\MAJP_personal\Masters_thesis\MastersMATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD094420-81EE-48E4-B702-44B8DB4555B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B5808B-1685-40AC-ABD8-CDA7BF7E6E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{B8F5F441-8AD5-44A2-8D30-C5B9926B48A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B8F5F441-8AD5-44A2-8D30-C5B9926B48A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,15 +28,10 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,7 +389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37F61A9-9295-4A3B-9C4C-1BB2C9658E63}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19:N20"/>
     </sheetView>
   </sheetViews>
@@ -921,4 +917,1266 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D212019-1F72-4790-B0B0-44C88418D0C6}">
+  <dimension ref="A1:AC14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>46</v>
+      </c>
+      <c r="D1">
+        <v>67</v>
+      </c>
+      <c r="E1">
+        <v>75</v>
+      </c>
+      <c r="F1">
+        <v>67</v>
+      </c>
+      <c r="G1">
+        <v>75</v>
+      </c>
+      <c r="H1">
+        <v>67</v>
+      </c>
+      <c r="I1">
+        <v>75</v>
+      </c>
+      <c r="J1">
+        <v>98</v>
+      </c>
+      <c r="K1">
+        <v>98</v>
+      </c>
+      <c r="L1">
+        <v>97</v>
+      </c>
+      <c r="M1">
+        <v>96</v>
+      </c>
+      <c r="N1">
+        <v>98</v>
+      </c>
+      <c r="O1">
+        <v>97</v>
+      </c>
+      <c r="P1">
+        <v>96</v>
+      </c>
+      <c r="Q1">
+        <v>96</v>
+      </c>
+      <c r="R1">
+        <v>99</v>
+      </c>
+      <c r="S1">
+        <v>99</v>
+      </c>
+      <c r="T1">
+        <v>96</v>
+      </c>
+      <c r="U1">
+        <v>97</v>
+      </c>
+      <c r="V1">
+        <v>97</v>
+      </c>
+      <c r="W1">
+        <v>97</v>
+      </c>
+      <c r="X1">
+        <v>98</v>
+      </c>
+      <c r="Y1">
+        <v>98</v>
+      </c>
+      <c r="Z1">
+        <v>98</v>
+      </c>
+      <c r="AA1">
+        <v>99</v>
+      </c>
+      <c r="AB1">
+        <v>97</v>
+      </c>
+      <c r="AC1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>73</v>
+      </c>
+      <c r="E2">
+        <v>72</v>
+      </c>
+      <c r="F2">
+        <v>73</v>
+      </c>
+      <c r="G2">
+        <v>72</v>
+      </c>
+      <c r="H2">
+        <v>73</v>
+      </c>
+      <c r="I2">
+        <v>72</v>
+      </c>
+      <c r="J2">
+        <v>96</v>
+      </c>
+      <c r="K2">
+        <v>97</v>
+      </c>
+      <c r="L2">
+        <v>94</v>
+      </c>
+      <c r="M2">
+        <v>96</v>
+      </c>
+      <c r="N2">
+        <v>93</v>
+      </c>
+      <c r="O2">
+        <v>93</v>
+      </c>
+      <c r="P2">
+        <v>96</v>
+      </c>
+      <c r="Q2">
+        <v>96</v>
+      </c>
+      <c r="R2">
+        <v>94</v>
+      </c>
+      <c r="S2">
+        <v>95</v>
+      </c>
+      <c r="T2">
+        <v>96</v>
+      </c>
+      <c r="U2">
+        <v>96</v>
+      </c>
+      <c r="V2">
+        <v>96</v>
+      </c>
+      <c r="W2">
+        <v>95</v>
+      </c>
+      <c r="X2">
+        <v>95</v>
+      </c>
+      <c r="Y2">
+        <v>95</v>
+      </c>
+      <c r="Z2">
+        <v>95</v>
+      </c>
+      <c r="AA2">
+        <v>94</v>
+      </c>
+      <c r="AB2">
+        <v>96</v>
+      </c>
+      <c r="AC2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>63</v>
+      </c>
+      <c r="D3">
+        <v>69</v>
+      </c>
+      <c r="E3">
+        <v>69</v>
+      </c>
+      <c r="F3">
+        <v>69</v>
+      </c>
+      <c r="G3">
+        <v>69</v>
+      </c>
+      <c r="H3">
+        <v>69</v>
+      </c>
+      <c r="I3">
+        <v>69</v>
+      </c>
+      <c r="J3">
+        <v>99</v>
+      </c>
+      <c r="K3">
+        <v>99</v>
+      </c>
+      <c r="L3">
+        <v>98</v>
+      </c>
+      <c r="M3">
+        <v>98</v>
+      </c>
+      <c r="N3">
+        <v>98</v>
+      </c>
+      <c r="O3">
+        <v>97</v>
+      </c>
+      <c r="P3">
+        <v>97</v>
+      </c>
+      <c r="Q3">
+        <v>97</v>
+      </c>
+      <c r="R3">
+        <v>96</v>
+      </c>
+      <c r="S3">
+        <v>96</v>
+      </c>
+      <c r="T3">
+        <v>97</v>
+      </c>
+      <c r="U3">
+        <v>97</v>
+      </c>
+      <c r="V3">
+        <v>99</v>
+      </c>
+      <c r="W3">
+        <v>100</v>
+      </c>
+      <c r="X3">
+        <v>100</v>
+      </c>
+      <c r="Y3">
+        <v>100</v>
+      </c>
+      <c r="Z3">
+        <v>98</v>
+      </c>
+      <c r="AA3">
+        <v>98</v>
+      </c>
+      <c r="AB3">
+        <v>96</v>
+      </c>
+      <c r="AC3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <v>79</v>
+      </c>
+      <c r="E4">
+        <v>79</v>
+      </c>
+      <c r="F4">
+        <v>79</v>
+      </c>
+      <c r="G4">
+        <v>79</v>
+      </c>
+      <c r="H4">
+        <v>79</v>
+      </c>
+      <c r="I4">
+        <v>79</v>
+      </c>
+      <c r="J4">
+        <v>100</v>
+      </c>
+      <c r="K4">
+        <v>99</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
+      </c>
+      <c r="M4">
+        <v>98</v>
+      </c>
+      <c r="N4">
+        <v>100</v>
+      </c>
+      <c r="O4">
+        <v>100</v>
+      </c>
+      <c r="P4">
+        <v>99</v>
+      </c>
+      <c r="Q4">
+        <v>99</v>
+      </c>
+      <c r="R4">
+        <v>100</v>
+      </c>
+      <c r="S4">
+        <v>99</v>
+      </c>
+      <c r="T4">
+        <v>99</v>
+      </c>
+      <c r="U4">
+        <v>99</v>
+      </c>
+      <c r="V4">
+        <v>100</v>
+      </c>
+      <c r="W4">
+        <v>100</v>
+      </c>
+      <c r="X4">
+        <v>98</v>
+      </c>
+      <c r="Y4">
+        <v>99</v>
+      </c>
+      <c r="Z4">
+        <v>100</v>
+      </c>
+      <c r="AA4">
+        <v>100</v>
+      </c>
+      <c r="AB4">
+        <v>99</v>
+      </c>
+      <c r="AC4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>69</v>
+      </c>
+      <c r="E5">
+        <v>70</v>
+      </c>
+      <c r="F5">
+        <v>69</v>
+      </c>
+      <c r="G5">
+        <v>70</v>
+      </c>
+      <c r="H5">
+        <v>69</v>
+      </c>
+      <c r="I5">
+        <v>70</v>
+      </c>
+      <c r="J5">
+        <v>94</v>
+      </c>
+      <c r="K5">
+        <v>99</v>
+      </c>
+      <c r="L5">
+        <v>98</v>
+      </c>
+      <c r="M5">
+        <v>99</v>
+      </c>
+      <c r="N5">
+        <v>98</v>
+      </c>
+      <c r="O5">
+        <v>99</v>
+      </c>
+      <c r="P5">
+        <v>99</v>
+      </c>
+      <c r="Q5">
+        <v>99</v>
+      </c>
+      <c r="R5">
+        <v>100</v>
+      </c>
+      <c r="S5">
+        <v>100</v>
+      </c>
+      <c r="T5">
+        <v>97</v>
+      </c>
+      <c r="U5">
+        <v>97</v>
+      </c>
+      <c r="V5">
+        <v>99</v>
+      </c>
+      <c r="W5">
+        <v>98</v>
+      </c>
+      <c r="X5">
+        <v>99</v>
+      </c>
+      <c r="Y5">
+        <v>99</v>
+      </c>
+      <c r="Z5">
+        <v>99</v>
+      </c>
+      <c r="AA5">
+        <v>99</v>
+      </c>
+      <c r="AB5">
+        <v>99</v>
+      </c>
+      <c r="AC5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>53</v>
+      </c>
+      <c r="E6">
+        <v>55</v>
+      </c>
+      <c r="F6">
+        <v>53</v>
+      </c>
+      <c r="G6">
+        <v>55</v>
+      </c>
+      <c r="H6">
+        <v>53</v>
+      </c>
+      <c r="I6">
+        <v>55</v>
+      </c>
+      <c r="J6">
+        <v>66</v>
+      </c>
+      <c r="K6">
+        <v>85</v>
+      </c>
+      <c r="L6">
+        <v>77</v>
+      </c>
+      <c r="M6">
+        <v>84</v>
+      </c>
+      <c r="N6">
+        <v>79</v>
+      </c>
+      <c r="O6">
+        <v>82</v>
+      </c>
+      <c r="P6">
+        <v>82</v>
+      </c>
+      <c r="Q6">
+        <v>85</v>
+      </c>
+      <c r="R6">
+        <v>84</v>
+      </c>
+      <c r="S6">
+        <v>84</v>
+      </c>
+      <c r="T6">
+        <v>82</v>
+      </c>
+      <c r="U6">
+        <v>82</v>
+      </c>
+      <c r="V6">
+        <v>80</v>
+      </c>
+      <c r="W6">
+        <v>80</v>
+      </c>
+      <c r="X6">
+        <v>80</v>
+      </c>
+      <c r="Y6">
+        <v>80</v>
+      </c>
+      <c r="Z6">
+        <v>80</v>
+      </c>
+      <c r="AA6">
+        <v>80</v>
+      </c>
+      <c r="AB6">
+        <v>80</v>
+      </c>
+      <c r="AC6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>41</v>
+      </c>
+      <c r="E7">
+        <v>43</v>
+      </c>
+      <c r="F7">
+        <v>41</v>
+      </c>
+      <c r="G7">
+        <v>42</v>
+      </c>
+      <c r="H7">
+        <v>41</v>
+      </c>
+      <c r="I7">
+        <v>43</v>
+      </c>
+      <c r="J7">
+        <v>52</v>
+      </c>
+      <c r="K7">
+        <v>65</v>
+      </c>
+      <c r="L7">
+        <v>60</v>
+      </c>
+      <c r="M7">
+        <v>65</v>
+      </c>
+      <c r="N7">
+        <v>61</v>
+      </c>
+      <c r="O7">
+        <v>65</v>
+      </c>
+      <c r="P7">
+        <v>66</v>
+      </c>
+      <c r="Q7">
+        <v>68</v>
+      </c>
+      <c r="R7">
+        <v>70</v>
+      </c>
+      <c r="S7">
+        <v>73</v>
+      </c>
+      <c r="T7">
+        <v>72</v>
+      </c>
+      <c r="U7">
+        <v>73</v>
+      </c>
+      <c r="V7">
+        <v>74</v>
+      </c>
+      <c r="W7">
+        <v>74</v>
+      </c>
+      <c r="X7">
+        <v>72</v>
+      </c>
+      <c r="Y7">
+        <v>74</v>
+      </c>
+      <c r="Z7">
+        <v>71</v>
+      </c>
+      <c r="AA7">
+        <v>73</v>
+      </c>
+      <c r="AB7">
+        <v>73</v>
+      </c>
+      <c r="AC7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>73</v>
+      </c>
+      <c r="E8">
+        <v>71</v>
+      </c>
+      <c r="F8">
+        <v>73</v>
+      </c>
+      <c r="G8">
+        <v>71</v>
+      </c>
+      <c r="H8">
+        <v>73</v>
+      </c>
+      <c r="I8">
+        <v>71</v>
+      </c>
+      <c r="J8">
+        <v>94</v>
+      </c>
+      <c r="K8">
+        <v>95</v>
+      </c>
+      <c r="L8">
+        <v>97</v>
+      </c>
+      <c r="M8">
+        <v>99</v>
+      </c>
+      <c r="N8">
+        <v>98</v>
+      </c>
+      <c r="O8">
+        <v>99</v>
+      </c>
+      <c r="P8">
+        <v>99</v>
+      </c>
+      <c r="Q8">
+        <v>99</v>
+      </c>
+      <c r="R8">
+        <v>99</v>
+      </c>
+      <c r="S8">
+        <v>99</v>
+      </c>
+      <c r="T8">
+        <v>98</v>
+      </c>
+      <c r="U8">
+        <v>99</v>
+      </c>
+      <c r="V8">
+        <v>98</v>
+      </c>
+      <c r="W8">
+        <v>97</v>
+      </c>
+      <c r="X8">
+        <v>100</v>
+      </c>
+      <c r="Y8">
+        <v>100</v>
+      </c>
+      <c r="Z8">
+        <v>100</v>
+      </c>
+      <c r="AA8">
+        <v>100</v>
+      </c>
+      <c r="AB8">
+        <v>99</v>
+      </c>
+      <c r="AC8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>71</v>
+      </c>
+      <c r="E9">
+        <v>73</v>
+      </c>
+      <c r="F9">
+        <v>71</v>
+      </c>
+      <c r="G9">
+        <v>73</v>
+      </c>
+      <c r="H9">
+        <v>71</v>
+      </c>
+      <c r="I9">
+        <v>73</v>
+      </c>
+      <c r="J9">
+        <v>96</v>
+      </c>
+      <c r="K9">
+        <v>99</v>
+      </c>
+      <c r="L9">
+        <v>98</v>
+      </c>
+      <c r="M9">
+        <v>98</v>
+      </c>
+      <c r="N9">
+        <v>99</v>
+      </c>
+      <c r="O9">
+        <v>99</v>
+      </c>
+      <c r="P9">
+        <v>98</v>
+      </c>
+      <c r="Q9">
+        <v>98</v>
+      </c>
+      <c r="R9">
+        <v>99</v>
+      </c>
+      <c r="S9">
+        <v>99</v>
+      </c>
+      <c r="T9">
+        <v>98</v>
+      </c>
+      <c r="U9">
+        <v>99</v>
+      </c>
+      <c r="V9">
+        <v>100</v>
+      </c>
+      <c r="W9">
+        <v>100</v>
+      </c>
+      <c r="X9">
+        <v>99</v>
+      </c>
+      <c r="Y9">
+        <v>99</v>
+      </c>
+      <c r="Z9">
+        <v>97</v>
+      </c>
+      <c r="AA9">
+        <v>97</v>
+      </c>
+      <c r="AB9">
+        <v>98</v>
+      </c>
+      <c r="AC9">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>79</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>51</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10">
+        <v>51</v>
+      </c>
+      <c r="H10">
+        <v>50</v>
+      </c>
+      <c r="I10">
+        <v>51</v>
+      </c>
+      <c r="J10">
+        <v>86</v>
+      </c>
+      <c r="K10">
+        <v>86</v>
+      </c>
+      <c r="L10">
+        <v>88</v>
+      </c>
+      <c r="M10">
+        <v>88</v>
+      </c>
+      <c r="N10">
+        <v>86</v>
+      </c>
+      <c r="O10">
+        <v>86</v>
+      </c>
+      <c r="P10">
+        <v>86</v>
+      </c>
+      <c r="Q10">
+        <v>84</v>
+      </c>
+      <c r="R10">
+        <v>88</v>
+      </c>
+      <c r="S10">
+        <v>89</v>
+      </c>
+      <c r="T10">
+        <v>84</v>
+      </c>
+      <c r="U10">
+        <v>85</v>
+      </c>
+      <c r="V10">
+        <v>85</v>
+      </c>
+      <c r="W10">
+        <v>83</v>
+      </c>
+      <c r="X10">
+        <v>80</v>
+      </c>
+      <c r="Y10">
+        <v>78</v>
+      </c>
+      <c r="Z10">
+        <v>80</v>
+      </c>
+      <c r="AA10">
+        <v>80</v>
+      </c>
+      <c r="AB10">
+        <v>79</v>
+      </c>
+      <c r="AC10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>69</v>
+      </c>
+      <c r="E11">
+        <v>71</v>
+      </c>
+      <c r="F11">
+        <v>69</v>
+      </c>
+      <c r="G11">
+        <v>71</v>
+      </c>
+      <c r="H11">
+        <v>69</v>
+      </c>
+      <c r="I11">
+        <v>71</v>
+      </c>
+      <c r="J11">
+        <v>95</v>
+      </c>
+      <c r="K11">
+        <v>95</v>
+      </c>
+      <c r="L11">
+        <v>97</v>
+      </c>
+      <c r="M11">
+        <v>97</v>
+      </c>
+      <c r="N11">
+        <v>95</v>
+      </c>
+      <c r="O11">
+        <v>95</v>
+      </c>
+      <c r="P11">
+        <v>94</v>
+      </c>
+      <c r="Q11">
+        <v>96</v>
+      </c>
+      <c r="R11">
+        <v>93</v>
+      </c>
+      <c r="S11">
+        <v>93</v>
+      </c>
+      <c r="T11">
+        <v>94</v>
+      </c>
+      <c r="U11">
+        <v>94</v>
+      </c>
+      <c r="V11">
+        <v>94</v>
+      </c>
+      <c r="W11">
+        <v>94</v>
+      </c>
+      <c r="X11">
+        <v>94</v>
+      </c>
+      <c r="Y11">
+        <v>94</v>
+      </c>
+      <c r="Z11">
+        <v>96</v>
+      </c>
+      <c r="AA11">
+        <v>96</v>
+      </c>
+      <c r="AB11">
+        <v>96</v>
+      </c>
+      <c r="AC11">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>31</v>
+      </c>
+      <c r="E12">
+        <v>31</v>
+      </c>
+      <c r="F12">
+        <v>31</v>
+      </c>
+      <c r="G12">
+        <v>31</v>
+      </c>
+      <c r="H12">
+        <v>31</v>
+      </c>
+      <c r="I12">
+        <v>31</v>
+      </c>
+      <c r="J12">
+        <v>48</v>
+      </c>
+      <c r="K12">
+        <v>49</v>
+      </c>
+      <c r="L12">
+        <v>48</v>
+      </c>
+      <c r="M12">
+        <v>49</v>
+      </c>
+      <c r="N12">
+        <v>50</v>
+      </c>
+      <c r="O12">
+        <v>49</v>
+      </c>
+      <c r="P12">
+        <v>47</v>
+      </c>
+      <c r="Q12">
+        <v>48</v>
+      </c>
+      <c r="R12">
+        <v>49</v>
+      </c>
+      <c r="S12">
+        <v>48</v>
+      </c>
+      <c r="T12">
+        <v>49</v>
+      </c>
+      <c r="U12">
+        <v>49</v>
+      </c>
+      <c r="V12">
+        <v>48</v>
+      </c>
+      <c r="W12">
+        <v>48</v>
+      </c>
+      <c r="X12">
+        <v>49</v>
+      </c>
+      <c r="Y12">
+        <v>49</v>
+      </c>
+      <c r="Z12">
+        <v>42</v>
+      </c>
+      <c r="AA12">
+        <v>42</v>
+      </c>
+      <c r="AB12">
+        <v>46</v>
+      </c>
+      <c r="AC12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>88</v>
+      </c>
+      <c r="K13">
+        <v>88</v>
+      </c>
+      <c r="L13">
+        <v>92</v>
+      </c>
+      <c r="M13">
+        <v>93</v>
+      </c>
+      <c r="N13">
+        <v>95</v>
+      </c>
+      <c r="O13">
+        <v>95</v>
+      </c>
+      <c r="P13">
+        <v>91</v>
+      </c>
+      <c r="Q13">
+        <v>91</v>
+      </c>
+      <c r="R13">
+        <v>94</v>
+      </c>
+      <c r="S13">
+        <v>95</v>
+      </c>
+      <c r="T13">
+        <v>93</v>
+      </c>
+      <c r="U13">
+        <v>94</v>
+      </c>
+      <c r="V13">
+        <v>98</v>
+      </c>
+      <c r="W13">
+        <v>97</v>
+      </c>
+      <c r="X13">
+        <v>96</v>
+      </c>
+      <c r="Y13">
+        <v>96</v>
+      </c>
+      <c r="Z13">
+        <v>95</v>
+      </c>
+      <c r="AA13">
+        <v>96</v>
+      </c>
+      <c r="AB13">
+        <v>94</v>
+      </c>
+      <c r="AC13">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>63</v>
+      </c>
+      <c r="E14">
+        <v>63</v>
+      </c>
+      <c r="F14">
+        <v>63</v>
+      </c>
+      <c r="G14">
+        <v>63</v>
+      </c>
+      <c r="H14">
+        <v>63</v>
+      </c>
+      <c r="I14">
+        <v>63</v>
+      </c>
+      <c r="J14">
+        <v>96</v>
+      </c>
+      <c r="K14">
+        <v>97</v>
+      </c>
+      <c r="L14">
+        <v>97</v>
+      </c>
+      <c r="M14">
+        <v>97</v>
+      </c>
+      <c r="N14">
+        <v>94</v>
+      </c>
+      <c r="O14">
+        <v>94</v>
+      </c>
+      <c r="P14">
+        <v>93</v>
+      </c>
+      <c r="Q14">
+        <v>92</v>
+      </c>
+      <c r="R14">
+        <v>94</v>
+      </c>
+      <c r="S14">
+        <v>92</v>
+      </c>
+      <c r="T14">
+        <v>94</v>
+      </c>
+      <c r="U14">
+        <v>92</v>
+      </c>
+      <c r="V14">
+        <v>95</v>
+      </c>
+      <c r="W14">
+        <v>95</v>
+      </c>
+      <c r="X14">
+        <v>96</v>
+      </c>
+      <c r="Y14">
+        <v>96</v>
+      </c>
+      <c r="Z14">
+        <v>96</v>
+      </c>
+      <c r="AA14">
+        <v>98</v>
+      </c>
+      <c r="AB14">
+        <v>95</v>
+      </c>
+      <c r="AC14">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>